<commit_message>
lots of simulation work
</commit_message>
<xml_diff>
--- a/tables/TableS7_simulated_bloom_design.xlsx
+++ b/tables/TableS7_simulated_bloom_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/domoic_acid_mgmt/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAE4E68-3E06-1D42-8074-060CBA1611CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD97BD36-6EB8-8547-A627-2B5681DB8775}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="7200" windowWidth="30420" windowHeight="15600" activeTab="1" xr2:uid="{8F65658D-0848-E744-8181-42A1E11BC0FA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{8F65658D-0848-E744-8181-42A1E11BC0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Formatted" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Bloom</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>span_y_hi</t>
+  </si>
+  <si>
+    <t>span_lo</t>
+  </si>
+  <si>
+    <t>span_hi</t>
   </si>
 </sst>
 </file>
@@ -599,258 +605,282 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36407D88-BFE0-8C4D-9C5C-0EAE5D42A991}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.1640625" customWidth="1"/>
+    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
       <c r="D2" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="F2" s="4">
         <v>25</v>
       </c>
-      <c r="E2" s="4">
+      <c r="G2" s="4">
         <v>50</v>
       </c>
-      <c r="F2" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.8</v>
-      </c>
       <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
         <v>0.3</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.4</v>
       </c>
       <c r="K2" s="5">
         <v>0.6</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="N2" s="4">
         <v>75</v>
       </c>
-      <c r="M2" s="6">
+      <c r="O2" s="6">
         <v>250</v>
       </c>
-      <c r="N2" s="6">
+      <c r="P2" s="6">
         <v>42.5</v>
       </c>
-      <c r="O2" s="6">
+      <c r="Q2" s="6">
         <v>45.5</v>
       </c>
-      <c r="P2" s="6">
+      <c r="R2" s="6">
         <v>10</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="S2" s="6">
         <v>40</v>
       </c>
-      <c r="R2" s="6">
+      <c r="T2" s="6">
         <v>1</v>
       </c>
-      <c r="S2" s="6">
+      <c r="U2" s="6">
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="F3" s="4">
+        <v>50</v>
+      </c>
+      <c r="G3" s="4">
+        <v>75</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="K3" s="5">
         <v>0.6</v>
       </c>
-      <c r="C3" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="L3" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="N3" s="5">
+        <v>100</v>
+      </c>
+      <c r="O3" s="5">
+        <v>250</v>
+      </c>
+      <c r="P3" s="6">
+        <v>42.5</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>45.5</v>
+      </c>
+      <c r="R3" s="6">
+        <v>10</v>
+      </c>
+      <c r="S3" s="6">
         <v>50</v>
       </c>
-      <c r="E3" s="4">
-        <v>75</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="L3" s="5">
-        <v>100</v>
-      </c>
-      <c r="M3" s="5">
-        <v>250</v>
-      </c>
-      <c r="N3" s="6">
-        <v>42.5</v>
-      </c>
-      <c r="O3" s="6">
-        <v>45.5</v>
-      </c>
-      <c r="P3" s="6">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>50</v>
-      </c>
-      <c r="R3" s="6">
+      <c r="T3" s="6">
         <v>1</v>
       </c>
-      <c r="S3" s="6">
+      <c r="U3" s="6">
         <v>2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="4">
-        <v>0.7</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="D4" s="3">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
         <v>75</v>
       </c>
-      <c r="E4" s="3">
+      <c r="G4" s="3">
         <v>125</v>
       </c>
-      <c r="F4" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="5">
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="M4" s="5">
         <v>0.8</v>
       </c>
-      <c r="H4" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="L4" s="5">
+      <c r="N4" s="5">
         <v>150</v>
       </c>
-      <c r="M4" s="5">
+      <c r="O4" s="5">
         <v>250</v>
       </c>
-      <c r="N4" s="6">
+      <c r="P4" s="6">
         <v>42.5</v>
       </c>
-      <c r="O4" s="6">
+      <c r="Q4" s="6">
         <v>45.5</v>
       </c>
-      <c r="P4" s="6">
+      <c r="R4" s="6">
         <v>10</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="S4" s="6">
         <v>60</v>
       </c>
-      <c r="R4" s="6">
+      <c r="T4" s="6">
         <v>1</v>
       </c>
-      <c r="S4" s="6">
+      <c r="U4" s="6">
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -863,8 +893,10 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -877,6 +909,8 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>